<commit_message>
Surat Keluar Panitia Fix
</commit_message>
<xml_diff>
--- a/Administrasi/Surat Keluar Panitia.xlsx
+++ b/Administrasi/Surat Keluar Panitia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="263">
   <si>
     <t>Nomor Surat</t>
   </si>
@@ -618,46 +618,226 @@
     <t>Pengantar LPJ</t>
   </si>
   <si>
-    <t>054/PAN.MUBES/HMJTI/XII/2021</t>
-  </si>
-  <si>
-    <t>055/PAN.MUBES/HMJTI/XII/2021</t>
-  </si>
-  <si>
-    <t>056/PAN.MUBES/HMJTI/XII/2021</t>
-  </si>
-  <si>
-    <t>057/PAN.MUBES/HMJTI/XII/2021</t>
-  </si>
-  <si>
-    <t>058/PAN.MUBES/HMJTI/XII/2021</t>
-  </si>
-  <si>
-    <t>059/PAN.MUBES/HMJTI/XII/2021</t>
-  </si>
-  <si>
-    <t>060/PAN.MUBES/HMJTI/XII/2021</t>
-  </si>
-  <si>
-    <t>061/PAN.MUBES/HMJTI/XII/2021</t>
-  </si>
-  <si>
-    <t>062/PAN.MUBES/HMJTI/XII/2021</t>
-  </si>
-  <si>
-    <t>063/PAN.MUBES/HMJTI/XII/2021</t>
-  </si>
-  <si>
-    <t>12 Desember 2021</t>
-  </si>
-  <si>
-    <t>MUBES</t>
-  </si>
-  <si>
-    <t>Jumat-sabtu, 24-25 Desember 2021</t>
-  </si>
-  <si>
-    <t>08.00 WIB-Selesai</t>
+    <t>012/A1/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>18 Desember 2021</t>
+  </si>
+  <si>
+    <t>TI Angkatan 2018(Reguler)</t>
+  </si>
+  <si>
+    <t>MUBES HMJTI</t>
+  </si>
+  <si>
+    <t>Jum’at-Sabtu,24-25 Desember 2021</t>
+  </si>
+  <si>
+    <t>07.30-Selesai</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gedung D </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Ruangan  302 &amp; 303</t>
+    </r>
+  </si>
+  <si>
+    <t>Undangan TI</t>
+  </si>
+  <si>
+    <t>013/A1/PAN.MUBES/HMJTI/XII/2022</t>
+  </si>
+  <si>
+    <t>TI Angkatan 2019(Reguler)</t>
+  </si>
+  <si>
+    <t>014/A1/PAN.MUBES/HMJTI/XII/2023</t>
+  </si>
+  <si>
+    <t>TI Angkatan 2020(Reguler)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gedung D </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Ruangan  302 &amp; 303</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>015/A1/PAN.MUBES/HMJTI/XII/2024</t>
+  </si>
+  <si>
+    <t>TI Angkatan 2021(Reguler)</t>
+  </si>
+  <si>
+    <t>016/A1/PAN.MUBES/HMJTI/XII/2025</t>
+  </si>
+  <si>
+    <t>TI Angkatan 2018(Karyawan)</t>
+  </si>
+  <si>
+    <t>017/A1/PAN.MUBES/HMJTI/XII/2026</t>
+  </si>
+  <si>
+    <t>TI Angkatan 2019(Karyawan)</t>
+  </si>
+  <si>
+    <t>018/A1/PAN.MUBES/HMJTI/XII/2027</t>
+  </si>
+  <si>
+    <t>TI Angkatan 2021(Karyawan)</t>
+  </si>
+  <si>
+    <t>019/A1/PAN.MUBES/HMJTI/XII/2028</t>
+  </si>
+  <si>
+    <t>Rito Cipta Sigitta Hariono, M.Kom</t>
+  </si>
+  <si>
+    <t>020/A1/PAN.MUBES/HMJTI/XII/2029</t>
+  </si>
+  <si>
+    <t>Undangan Ketua BEM FST</t>
+  </si>
+  <si>
+    <t>021/A1/PAN.MUBES/HMJTI/XII/2030</t>
+  </si>
+  <si>
+    <t>Saktiningrum Nikmatul Khoiriyah</t>
+  </si>
+  <si>
+    <t>Undangan Ketua BEM UP</t>
+  </si>
+  <si>
+    <t>022/A1/PAN.MUBES/HMJTI/XII/2031</t>
+  </si>
+  <si>
+    <t>Khornelis Anjelina</t>
+  </si>
+  <si>
+    <t>Undangan Ketua DPM UP</t>
+  </si>
+  <si>
+    <t>023/A1/PAN.MUBES/HMJTI/XII/2032</t>
+  </si>
+  <si>
+    <t>Teguh Adi Nugroho, M.Kom</t>
+  </si>
+  <si>
+    <t>024/A1/PAN.MUBES/HMJTI/XII/2033</t>
+  </si>
+  <si>
+    <t>025/A1/PAN.MUBES/HMJTI/XII/2034</t>
+  </si>
+  <si>
+    <t>Sidik Agus Triyono</t>
+  </si>
+  <si>
+    <t>026/A1/PAN.MUBES/HMJTI/XII/2035</t>
+  </si>
+  <si>
+    <t>027/A1/PAN.MUBES/HMJTI/XII/2035</t>
+  </si>
+  <si>
+    <t>22 Desember 2021</t>
+  </si>
+  <si>
+    <t>Atik Syaiful Rohman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undangan </t>
+  </si>
+  <si>
+    <t>054/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>MUBES HMJTI 2021</t>
+  </si>
+  <si>
+    <t>Jum'at - Sabtu, 24-25 Desember 2021</t>
+  </si>
+  <si>
+    <t>08.00 WIB - Selesai</t>
+  </si>
+  <si>
+    <t>Ruangan D 302</t>
+  </si>
+  <si>
+    <t>055/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>056/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>057/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>058/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>059/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>060/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>061/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>062/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>063/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>064/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>065/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>066/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>067/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>068/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>069/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>070/A3/PAN.MUBES/HMJTI/XII/2021</t>
+  </si>
+  <si>
+    <t>071/A3/PAN.MUBES/HMJTI/XII/2021</t>
   </si>
 </sst>
 </file>
@@ -667,7 +847,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -693,6 +873,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -714,7 +922,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -739,6 +947,17 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1044,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1517,6 +1736,518 @@
       </c>
       <c r="M12" s="2" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2378,10 +3109,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4012,293 +4743,579 @@
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>200</v>
+      <c r="A48" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>210</v>
+        <v>109</v>
+      </c>
+      <c r="C48" s="12">
+        <v>44542</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>115</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>212</v>
+        <v>242</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>213</v>
+        <v>244</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="M48" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>201</v>
+      <c r="A49" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E49" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" s="12">
+        <v>44542</v>
+      </c>
+      <c r="E49" s="17" t="s">
         <v>125</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>212</v>
+        <v>242</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>213</v>
+        <v>244</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="M49" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>202</v>
+      <c r="A50" s="2" t="s">
+        <v>247</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E50" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="12">
+        <v>44542</v>
+      </c>
+      <c r="E50" s="17" t="s">
         <v>43</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>212</v>
+        <v>242</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>213</v>
+        <v>244</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="M50" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>203</v>
+      <c r="A51" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E51" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="12">
+        <v>44542</v>
+      </c>
+      <c r="E51" s="17" t="s">
         <v>118</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>212</v>
+        <v>242</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>213</v>
+        <v>244</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="M51" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>204</v>
+      <c r="A52" s="2" t="s">
+        <v>249</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E52" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" s="12">
+        <v>44542</v>
+      </c>
+      <c r="E52" s="17" t="s">
         <v>119</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>212</v>
+        <v>242</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>213</v>
+        <v>244</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="M52" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>205</v>
+      <c r="A53" s="2" t="s">
+        <v>250</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E53" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="12">
+        <v>44542</v>
+      </c>
+      <c r="E53" s="17" t="s">
         <v>120</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>212</v>
+        <v>242</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>213</v>
+        <v>244</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="M53" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>206</v>
+      <c r="A54" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E54" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="12">
+        <v>44542</v>
+      </c>
+      <c r="E54" s="17" t="s">
         <v>191</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>212</v>
+        <v>242</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>213</v>
+        <v>244</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="M54" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>207</v>
+      <c r="A55" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E55" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" s="12">
+        <v>44542</v>
+      </c>
+      <c r="E55" s="17" t="s">
         <v>192</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>212</v>
+        <v>242</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>213</v>
+        <v>244</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="M55" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>208</v>
+      <c r="A56" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E56" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="12">
+        <v>44542</v>
+      </c>
+      <c r="E56" s="17" t="s">
         <v>44</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>212</v>
+        <v>242</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>213</v>
+        <v>244</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="M56" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>209</v>
+      <c r="A57" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E57" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="12">
+        <v>44542</v>
+      </c>
+      <c r="E57" s="17" t="s">
         <v>126</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>212</v>
+        <v>242</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>213</v>
+        <v>244</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="M57" s="7" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C58" s="12">
+        <v>44559</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="J58" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="M58" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C59" s="12">
+        <v>44559</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="M59" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C60" s="12">
+        <v>44559</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="J60" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="M60" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C61" s="12">
+        <v>44559</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="J61" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="M61" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C62" s="12">
+        <v>44559</v>
+      </c>
+      <c r="E62" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H62" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="J62" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="M62" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C63" s="12">
+        <v>44559</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="J63" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="M63" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C64" s="12">
+        <v>44559</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H64" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="J64" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="M64" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C65" s="12">
+        <v>44559</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="J65" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="M65" s="7" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>